<commit_message>
Perform Operation Using Pandas
</commit_message>
<xml_diff>
--- a/Pandas/examples/ex1.xlsx
+++ b/Pandas/examples/ex1.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Unnamed: 0</t>
+  </si>
   <si>
     <t>a</t>
   </si>
@@ -402,24 +405,27 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
@@ -435,11 +441,11 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
@@ -455,11 +461,11 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
@@ -475,7 +481,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>